<commit_message>
added lists with DO data
</commit_message>
<xml_diff>
--- a/PPU/LAB1/data.xlsx
+++ b/PPU/LAB1/data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\University\PPU\LAB1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0900B930-79AF-4F1E-8FF3-B237458F8E2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -141,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -453,18 +447,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +527,14 @@
         <v>20</v>
       </c>
       <c r="H2">
-        <v>146.6</v>
+        <f>J2/2</f>
+        <v>73.3</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
+      </c>
+      <c r="J2">
+        <v>146.6</v>
       </c>
       <c r="K2">
         <f>K1/L1</f>
@@ -547,6 +545,10 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H9" si="0">J3/2</f>
+        <v>0</v>
+      </c>
       <c r="K3">
         <f>$K$2*L3</f>
         <v>133.33333333333331</v>
@@ -577,11 +579,15 @@
       <c r="G4" s="2">
         <v>11</v>
       </c>
-      <c r="H4" s="2">
-        <v>120</v>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="J4" s="2">
+        <v>120</v>
       </c>
       <c r="K4">
         <f>$K$2*L4</f>
@@ -614,10 +620,14 @@
         <v>22.5</v>
       </c>
       <c r="H5">
-        <v>146.6</v>
+        <f t="shared" si="0"/>
+        <v>73.3</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
+      </c>
+      <c r="J5">
+        <v>146.6</v>
       </c>
       <c r="K5">
         <f>$K$2*L5</f>
@@ -649,11 +659,15 @@
       <c r="G6" s="2">
         <v>15</v>
       </c>
-      <c r="H6" s="2">
-        <v>120</v>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="J6" s="2">
+        <v>120</v>
       </c>
       <c r="K6">
         <f>$K$2*L6</f>
@@ -686,10 +700,14 @@
         <v>25</v>
       </c>
       <c r="H7">
-        <v>140</v>
+        <f t="shared" si="0"/>
+        <v>70</v>
       </c>
       <c r="I7" t="s">
         <v>23</v>
+      </c>
+      <c r="J7">
+        <v>140</v>
       </c>
       <c r="K7">
         <f>$K$2*L7</f>
@@ -721,11 +739,15 @@
       <c r="G8" s="2">
         <v>20.5</v>
       </c>
-      <c r="H8" s="2">
-        <v>146.6</v>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>73.3</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="J8" s="2">
+        <v>146.6</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -751,10 +773,14 @@
         <v>20.5</v>
       </c>
       <c r="H9">
-        <v>160</v>
+        <f t="shared" si="0"/>
+        <v>80</v>
       </c>
       <c r="I9" t="s">
         <v>23</v>
+      </c>
+      <c r="J9">
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -832,7 +858,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -852,7 +878,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -872,7 +898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -892,7 +918,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -910,6 +936,70 @@
       </c>
       <c r="F20" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+      <c r="G26">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>